<commit_message>
update weight with images
</commit_message>
<xml_diff>
--- a/tracking/daily_tracking.xlsx
+++ b/tracking/daily_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\JJBaby\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1210905E-AAEA-41D5-84F9-51F0AF6E8055}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBA5B64-D2E5-43EB-9C33-FFEFA0BC3BFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5A54F73C-E4A4-488F-8451-B849D94644A9}"/>
   </bookViews>
@@ -718,13 +718,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBB36FB-D2CE-4C1B-BDC8-34816EBD3834}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,7 +833,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <f t="shared" ref="A5:A43" si="2">A4+7</f>
+        <f t="shared" ref="A5:A47" si="2">A4+7</f>
         <v>43489</v>
       </c>
       <c r="B5" s="2">
@@ -961,14 +961,14 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E10" s="7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" si="0"/>
-        <v>60.1</v>
+        <v>60.2</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" si="1"/>
@@ -1914,10 +1914,18 @@
       <c r="G39" s="1">
         <v>60</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
+      <c r="H39" s="1">
+        <v>60.1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>60.1</v>
+      </c>
+      <c r="J39" s="1">
+        <v>60.3</v>
+      </c>
+      <c r="K39" s="1">
+        <v>60.3</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
@@ -1927,21 +1935,35 @@
       <c r="B40" s="1">
         <v>37</v>
       </c>
-      <c r="C40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D40" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>60.4</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="E40" s="7">
+        <v>60.1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>60.4</v>
+      </c>
+      <c r="G40" s="1">
+        <v>60.5</v>
+      </c>
+      <c r="H40" s="1">
+        <v>60.7</v>
+      </c>
+      <c r="I40" s="1">
+        <v>60.8</v>
+      </c>
+      <c r="J40" s="1">
+        <v>60.2</v>
+      </c>
+      <c r="K40" s="1">
+        <v>60.1</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
@@ -1951,21 +1973,35 @@
       <c r="B41" s="2">
         <v>38</v>
       </c>
-      <c r="C41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D41" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>60.7</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="E41" s="7">
+        <v>60.3</v>
+      </c>
+      <c r="F41" s="1">
+        <v>60.9</v>
+      </c>
+      <c r="G41" s="1">
+        <v>60.9</v>
+      </c>
+      <c r="H41" s="1">
+        <v>60.9</v>
+      </c>
+      <c r="I41" s="1">
+        <v>60.8</v>
+      </c>
+      <c r="J41" s="1">
+        <v>60.7</v>
+      </c>
+      <c r="K41" s="1">
+        <v>60.5</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
@@ -1975,15 +2011,17 @@
       <c r="B42" s="1">
         <v>39</v>
       </c>
-      <c r="C42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>61</v>
       </c>
       <c r="D42" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E42" s="7"/>
+      <c r="E42" s="7">
+        <v>61</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -2015,6 +2053,30 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <f t="shared" si="2"/>
+        <v>43762</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
+        <f t="shared" si="2"/>
+        <v>43769</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <f t="shared" si="2"/>
+        <v>43776</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <f t="shared" si="2"/>
+        <v>43783</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update weight excel file
</commit_message>
<xml_diff>
--- a/tracking/daily_tracking.xlsx
+++ b/tracking/daily_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\JJBaby\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA7326D-A317-4047-B6B7-3A97D5681474}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8FEBD-BCB3-4B3F-8FFC-9A97619FC4C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5A54F73C-E4A4-488F-8451-B849D94644A9}"/>
   </bookViews>
@@ -721,10 +721,10 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
+      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C42" s="2">
         <f t="shared" si="0"/>
-        <v>61.2</v>
+        <v>61.1</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E42" s="7">
         <v>61</v>
@@ -2028,10 +2028,18 @@
       <c r="G42" s="1">
         <v>61.2</v>
       </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="H42" s="1">
+        <v>61.1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>61.3</v>
+      </c>
+      <c r="J42" s="1">
+        <v>61.1</v>
+      </c>
+      <c r="K42" s="1">
+        <v>61</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
@@ -2041,15 +2049,17 @@
       <c r="B43" s="2">
         <v>40</v>
       </c>
-      <c r="C43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>61</v>
       </c>
       <c r="D43" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E43" s="7"/>
+      <c r="E43" s="7">
+        <v>61</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>

</xml_diff>